<commit_message>
matrix plot rebuild with Labeled_Matrix object and hypoxanthine labeling
</commit_message>
<xml_diff>
--- a/pytheas_data/nucleotide_table.xlsx
+++ b/pytheas_data/nucleotide_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrwill/prog/Pytheas_Folder/Pytheas_Qt_root/Pytheas_Qt/pytheas_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA2267C-DF2F-C346-9F5E-EEF636F2837A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56D0AB5-A540-E84A-97E0-63943BE68A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7400" yWindow="720" windowWidth="39180" windowHeight="25200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="760" windowWidth="28580" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="551">
   <si>
     <t>Name</t>
   </si>
@@ -1670,6 +1670,9 @@
   </si>
   <si>
     <t>NNN</t>
+  </si>
+  <si>
+    <t>non</t>
   </si>
 </sst>
 </file>
@@ -2039,8 +2042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="O114" sqref="O114"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2106,6 +2109,9 @@
       <c r="F2">
         <v>65</v>
       </c>
+      <c r="G2" t="s">
+        <v>129</v>
+      </c>
       <c r="H2" t="s">
         <v>482</v>
       </c>
@@ -2135,6 +2141,9 @@
       <c r="F3">
         <v>67</v>
       </c>
+      <c r="G3" t="s">
+        <v>130</v>
+      </c>
       <c r="H3" t="s">
         <v>482</v>
       </c>
@@ -2164,6 +2173,9 @@
       <c r="F4">
         <v>71</v>
       </c>
+      <c r="G4" t="s">
+        <v>131</v>
+      </c>
       <c r="H4" t="s">
         <v>482</v>
       </c>
@@ -2193,6 +2205,9 @@
       <c r="F5">
         <v>85</v>
       </c>
+      <c r="G5" t="s">
+        <v>132</v>
+      </c>
       <c r="H5" t="s">
         <v>482</v>
       </c>
@@ -5370,6 +5385,9 @@
       <c r="D113" t="s">
         <v>383</v>
       </c>
+      <c r="G113" t="s">
+        <v>493</v>
+      </c>
       <c r="H113" t="s">
         <v>484</v>
       </c>
@@ -5393,6 +5411,9 @@
       <c r="D114" t="s">
         <v>384</v>
       </c>
+      <c r="G114" t="s">
+        <v>493</v>
+      </c>
       <c r="H114" t="s">
         <v>484</v>
       </c>
@@ -5416,6 +5437,9 @@
       <c r="D115" t="s">
         <v>383</v>
       </c>
+      <c r="G115" t="s">
+        <v>550</v>
+      </c>
       <c r="H115" t="s">
         <v>485</v>
       </c>
@@ -5439,6 +5463,9 @@
       <c r="D116" t="s">
         <v>384</v>
       </c>
+      <c r="G116" t="s">
+        <v>493</v>
+      </c>
       <c r="H116" t="s">
         <v>485</v>
       </c>
@@ -5462,6 +5489,9 @@
       <c r="D117" t="s">
         <v>385</v>
       </c>
+      <c r="G117" t="s">
+        <v>493</v>
+      </c>
       <c r="H117" t="s">
         <v>485</v>
       </c>
@@ -5505,6 +5535,9 @@
       <c r="D119" t="s">
         <v>387</v>
       </c>
+      <c r="G119" t="s">
+        <v>130</v>
+      </c>
       <c r="H119" t="s">
         <v>485</v>
       </c>
@@ -5525,6 +5558,9 @@
       <c r="D120" t="s">
         <v>388</v>
       </c>
+      <c r="G120" t="s">
+        <v>130</v>
+      </c>
       <c r="H120" t="s">
         <v>485</v>
       </c>
@@ -5545,6 +5581,9 @@
       <c r="D121" t="s">
         <v>389</v>
       </c>
+      <c r="G121" t="s">
+        <v>130</v>
+      </c>
       <c r="H121" t="s">
         <v>485</v>
       </c>
@@ -5565,6 +5604,9 @@
       <c r="D122" t="s">
         <v>390</v>
       </c>
+      <c r="G122" t="s">
+        <v>130</v>
+      </c>
       <c r="H122" t="s">
         <v>485</v>
       </c>
@@ -5585,6 +5627,9 @@
       <c r="D123" t="s">
         <v>542</v>
       </c>
+      <c r="G123" t="s">
+        <v>493</v>
+      </c>
       <c r="H123" t="s">
         <v>543</v>
       </c>
@@ -5605,6 +5650,9 @@
       <c r="D124" t="s">
         <v>545</v>
       </c>
+      <c r="G124" t="s">
+        <v>493</v>
+      </c>
       <c r="H124" t="s">
         <v>543</v>
       </c>
@@ -5625,6 +5673,9 @@
       <c r="D125" t="s">
         <v>547</v>
       </c>
+      <c r="G125" t="s">
+        <v>493</v>
+      </c>
       <c r="H125" t="s">
         <v>543</v>
       </c>
@@ -5644,6 +5695,9 @@
       </c>
       <c r="D126" t="s">
         <v>549</v>
+      </c>
+      <c r="G126" t="s">
+        <v>493</v>
       </c>
       <c r="H126" t="s">
         <v>543</v>

</xml_diff>